<commit_message>
Update Autographen_Autoren geändert oder neu.xlsx
</commit_message>
<xml_diff>
--- a/excel/Autographen_Autoren geändert oder neu.xlsx
+++ b/excel/Autographen_Autoren geändert oder neu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b1039121\Desktop\Las_diverses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b1039121\Documents\GitHub\SZD\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="170">
   <si>
     <t>Normalisiert (nach GND)</t>
   </si>
@@ -564,41 +564,28 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val="Calibri (Textkörper)_x0000_"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>Joseph</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Leoncavallo, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Textkörper)_x0000_"/>
-      </rPr>
-      <t>Ruggiero</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rossini, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Textkörper)_x0000_"/>
-      </rPr>
-      <t>Gioachino</t>
-    </r>
+    <t>Leoncavallo, Ruggiero</t>
+  </si>
+  <si>
+    <t>Lanner, Joseph</t>
+  </si>
+  <si>
+    <t>Rossini, Gioachino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -641,10 +628,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri (Textkörper)_x0000_"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1024,11 +1007,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
     <col min="2" max="2" width="30.796875" bestFit="1" customWidth="1"/>
@@ -1036,7 +1019,7 @@
     <col min="4" max="4" width="76.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1064,7 +1047,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1061,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1092,7 +1075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1089,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1148,7 +1131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1162,7 +1145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1176,7 +1159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1190,7 +1173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1204,7 +1187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1218,7 +1201,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1215,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1246,7 +1229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1260,7 +1243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1274,7 +1257,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1288,7 +1271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1302,7 +1285,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1316,7 +1299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1330,7 +1313,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1344,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1358,7 +1341,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1372,7 +1355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1386,7 +1369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1400,7 +1383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1414,7 +1397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1428,7 +1411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1442,7 +1425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1456,7 +1439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1470,7 +1453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1484,7 +1467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21">
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="10" t="s">
         <v>67</v>
       </c>
@@ -1492,7 +1475,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" ht="21">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
@@ -1506,7 +1489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1520,7 +1503,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1534,7 +1517,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1548,7 +1531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1562,7 +1545,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1576,7 +1559,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -1590,7 +1573,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -1604,7 +1587,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -1618,7 +1601,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -1632,7 +1615,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1646,7 +1629,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -1660,7 +1643,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -1674,7 +1657,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -1688,7 +1671,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -1702,7 +1685,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -1716,7 +1699,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -1730,7 +1713,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -1744,7 +1727,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -1758,7 +1741,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -1772,7 +1755,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -1780,13 +1763,13 @@
         <v>166</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -1800,7 +1783,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -1814,7 +1797,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -1828,7 +1811,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -1842,7 +1825,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -1856,7 +1839,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -1870,21 +1853,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>94</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -1898,7 +1881,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -1912,7 +1895,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -1926,7 +1909,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>138</v>
       </c>
@@ -1940,7 +1923,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -1954,7 +1937,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -1968,7 +1951,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>145</v>
       </c>
@@ -1982,7 +1965,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>148</v>
       </c>
@@ -1996,7 +1979,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>150</v>
       </c>
@@ -2010,7 +1993,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>152</v>
       </c>
@@ -2024,7 +2007,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>154</v>
       </c>

</xml_diff>